<commit_message>
creacion de teclado ocn pausa
</commit_message>
<xml_diff>
--- a/BOLERA-FACTURA/BOLETA HOY.xlsx
+++ b/BOLERA-FACTURA/BOLETA HOY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\BOLERA-FACTURA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\EXTENCION_PHYTON\BOLERA-FACTURA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D236531C-D353-498A-8334-2F35CCA3DED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD286D3-EBCD-4D7A-A1B1-BB4E8AB65FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   BOLERA-FACTURA/BOLETA HOY.xlsx 	modified:   BOLERA-FACTURA/FORMATO PARA LLENADO DE FACTURAS Y BOLETAS - VILLAFUERTE - 5 ESQUINAS.xlsx 	modified:   BOLERA-FACTURA/FORMATO PARA LLENADO DE FACTURAS Y BOLETAS EMITIDAS - SOLUCIONES - 5 ESQUINAS.xlsx 	modified:   boleta factura-teclado/boleta teclado.py
</commit_message>
<xml_diff>
--- a/BOLERA-FACTURA/BOLETA HOY.xlsx
+++ b/BOLERA-FACTURA/BOLETA HOY.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\EXTENCION_PHYTON\BOLERA-FACTURA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD286D3-EBCD-4D7A-A1B1-BB4E8AB65FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222C843F-D36C-4D29-806F-8513EFC9E2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,63 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
-  <si>
-    <t>VERZUS X 100GR</t>
-  </si>
-  <si>
-    <t>BUKRA 580 WG X 100GR</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+  <si>
+    <t>unidad</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>IGV</t>
+  </si>
+  <si>
+    <t>SENSEI 350 SC X 1LT</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>CRUCIAL FS X 250ML</t>
+  </si>
+  <si>
+    <t>SELLADOR 400 EC X 1LT</t>
+  </si>
+  <si>
+    <t>FARMOZINE X 1LT</t>
   </si>
   <si>
     <t>ROUNDUP SL X 1LT</t>
-  </si>
-  <si>
-    <t>MERIDIAN X 100GR</t>
-  </si>
-  <si>
-    <t>KUROMIL 90P BOL 100GRS</t>
-  </si>
-  <si>
-    <t>DELTAPLUS 2.5 EC X 1LT</t>
-  </si>
-  <si>
-    <t>SENSEI 350 SC X 1LT</t>
-  </si>
-  <si>
-    <t>HOOK X 200GR</t>
-  </si>
-  <si>
-    <t>FARMOZINE X 1LT</t>
-  </si>
-  <si>
-    <t>EMBATE 480 SL X 1LT</t>
-  </si>
-  <si>
-    <t>TIFON 4E X 1LT</t>
-  </si>
-  <si>
-    <t>KIETO 150 WG X 100GR</t>
-  </si>
-  <si>
-    <t>SKIRLA X 100GR</t>
-  </si>
-  <si>
-    <t>LOVERA X 1LT</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>unidad</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>IGV</t>
   </si>
 </sst>
 </file>
@@ -399,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,212 +386,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
         <v>5</v>
-      </c>
-      <c r="C7">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>110</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>